<commit_message>
detalhamento caso de uso
</commit_message>
<xml_diff>
--- a/documentacao/Documentos de caso de uso.xlsx
+++ b/documentacao/Documentos de caso de uso.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b505be104808171/Documentos/Eng_software/semestre_2/Diagramas/06-09-22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDUARDO\Desktop\Brechó\Projeto-integrador-G7\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{379C491F-11F1-45CF-A2A3-B86CAB48B18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65B12FA8-8B91-4471-AD97-214D8B3C3B6A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="124">
   <si>
     <t>C001</t>
   </si>
@@ -316,12 +315,93 @@
   </si>
   <si>
     <t>DOCUMENTAÇÃO DOS CASOS DE USO</t>
+  </si>
+  <si>
+    <t>O sistema leva para tela do item selecionado</t>
+  </si>
+  <si>
+    <t>Clicou no menu</t>
+  </si>
+  <si>
+    <t>O sistema leva para a tela home</t>
+  </si>
+  <si>
+    <t>Clicou na logo</t>
+  </si>
+  <si>
+    <t>O sistema leva o cliente para tela da lista de desejo, com o produto inserido</t>
+  </si>
+  <si>
+    <t>Clicou para adicionar na lista de desejo</t>
+  </si>
+  <si>
+    <t>O sistema leva o cliente para tela do carrinho com o produto inserido</t>
+  </si>
+  <si>
+    <t>Clicou para adicionar no carrinho</t>
+  </si>
+  <si>
+    <t>2 - O sistema irá abrir a tela de detalhe do produto</t>
+  </si>
+  <si>
+    <t>1 - Usuário clicou no produto para saber mais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizar o detalhe do produto </t>
+  </si>
+  <si>
+    <t>Cliente/Administrador</t>
+  </si>
+  <si>
+    <t>O usuário vai saber mais sobre o produto que ele deseja nessa tela</t>
+  </si>
+  <si>
+    <t>Tela de Detalhe do Produto</t>
+  </si>
+  <si>
+    <t>9- Sistema verifica os dados e redireciona para pagina de cadastro de produtos</t>
+  </si>
+  <si>
+    <t>7- Usuário clicou no botão entrar</t>
+  </si>
+  <si>
+    <t>6 - Sistema redireciona para o botão entrar</t>
+  </si>
+  <si>
+    <t>5- Usuário digitou a senha</t>
+  </si>
+  <si>
+    <t>4- Direciona para o usuário digitar a senha</t>
+  </si>
+  <si>
+    <t>3 - Usuário digiou o login</t>
+  </si>
+  <si>
+    <t>2 - Sistema abriu a opção para o usuário digitar o login</t>
+  </si>
+  <si>
+    <t>1- Usuário clicou no campo de login</t>
+  </si>
+  <si>
+    <t>Acessar cadastro de novos produtos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efetuar Login </t>
+  </si>
+  <si>
+    <t>Login Administrador</t>
+  </si>
+  <si>
+    <t>C005</t>
+  </si>
+  <si>
+    <t>C006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -508,62 +588,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,159 +925,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="53" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="C9" s="22"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -1022,7 +1099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -1033,7 +1110,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -1044,7 +1121,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -1055,7 +1132,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>3</v>
       </c>
@@ -1066,14 +1143,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
@@ -1084,7 +1161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -1095,129 +1172,129 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="22"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="17"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="17"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="17"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>10</v>
       </c>
@@ -1228,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>1</v>
       </c>
@@ -1239,7 +1316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>1</v>
       </c>
@@ -1250,7 +1327,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -1261,14 +1338,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -1290,269 +1367,269 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="17"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="17"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="22"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="17"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="17"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="22"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="17"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="17"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="C59" s="22"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="18"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="17"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="17"/>
+      <c r="B63" s="22"/>
       <c r="C63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="17"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="23"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="17"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="17"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="22"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="17"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="22"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="17"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="22"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="17"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="22"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C75" s="17"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="18" t="s">
+      <c r="C75" s="22"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="18"/>
+      <c r="B77" s="26"/>
       <c r="C77" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="17"/>
+      <c r="B78" s="22"/>
       <c r="C78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
       <c r="C79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="17"/>
+      <c r="B80" s="22"/>
       <c r="C80" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="32"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="20" t="s">
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
         <v>10</v>
       </c>
@@ -1563,7 +1640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>4</v>
       </c>
@@ -1574,7 +1651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>4</v>
       </c>
@@ -1585,7 +1662,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>4</v>
       </c>
@@ -1596,7 +1673,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>89</v>
       </c>
@@ -1607,14 +1684,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>10</v>
       </c>
@@ -1625,7 +1702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="14">
         <v>3</v>
       </c>
@@ -1636,7 +1713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>7</v>
       </c>
@@ -1647,35 +1724,453 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
-      <c r="B93" s="23"/>
-      <c r="C93" s="23"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
-      <c r="B94" s="24"/>
-      <c r="C94" s="24"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="33"/>
-      <c r="B96" s="33"/>
-      <c r="C96" s="33"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="34"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="17"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95" s="22"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C97" s="22"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="26"/>
+      <c r="C101" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="22"/>
+      <c r="C102" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103" s="22"/>
+      <c r="C103" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="22"/>
+      <c r="C104" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105" s="22"/>
+      <c r="C105" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B106" s="27"/>
+      <c r="C106" s="27"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="2"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="2"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="2"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="2"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="2"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="30"/>
+      <c r="C114" s="31"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="2"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="2"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="18"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="18"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B119" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C119" s="22"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C120" s="22"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C121" s="22"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C122" s="22"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C123" s="22"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C124" s="22"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="26"/>
+      <c r="C125" s="26"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="26"/>
+      <c r="C126" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B127" s="22"/>
+      <c r="C127" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="22"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B129" s="27"/>
+      <c r="C129" s="27"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>1</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>1</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>1</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>1</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="2"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B137" s="30"/>
+      <c r="C137" s="31"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="2"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
+  <mergeCells count="88">
+    <mergeCell ref="A130:C130"/>
+    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A107:C107"/>
+    <mergeCell ref="A114:C114"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A50:C53"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A27:C30"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="A66:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A93:C96"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="B71:C71"/>
@@ -1689,52 +2184,7 @@
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A66:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A27:C30"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A50:C53"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="B94:C94"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajustado caso de uso
</commit_message>
<xml_diff>
--- a/documentacao/Documentos de caso de uso.xlsx
+++ b/documentacao/Documentos de caso de uso.xlsx
@@ -344,9 +344,6 @@
     <t>2 - O sistema irá abrir a tela de detalhe do produto</t>
   </si>
   <si>
-    <t>1 - Usuário clicou no produto para saber mais</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vizualizar o detalhe do produto </t>
   </si>
   <si>
@@ -396,13 +393,16 @@
   </si>
   <si>
     <t>C006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Usuário clicou no produto para ver detalhe </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +437,14 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -538,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -597,14 +605,44 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -612,35 +650,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A111" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="K110" sqref="K110"/>
+      <selection activeCell="L132" sqref="L132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,39 +952,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -982,16 +993,16 @@
       <c r="B6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
@@ -1000,75 +1011,75 @@
       <c r="B8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
@@ -1144,11 +1155,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -1173,42 +1184,42 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="23"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="22"/>
+      <c r="C32" s="23"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
@@ -1217,75 +1228,75 @@
       <c r="B33" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="22"/>
+      <c r="C34" s="23"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="23"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="26"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
@@ -1368,42 +1379,42 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="22"/>
+      <c r="C54" s="23"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="22"/>
+      <c r="C55" s="23"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -1412,122 +1423,122 @@
       <c r="B56" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="22"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="22"/>
+      <c r="C57" s="23"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="22"/>
+      <c r="C58" s="23"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="22"/>
+      <c r="C59" s="23"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="26"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="22"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="22"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="21"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="21"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="22"/>
+      <c r="C70" s="23"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="22"/>
+      <c r="C71" s="23"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
@@ -1536,91 +1547,91 @@
       <c r="B72" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="22"/>
+      <c r="C72" s="23"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="22"/>
+      <c r="C73" s="23"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="22"/>
+      <c r="C74" s="23"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C75" s="22"/>
+      <c r="C75" s="23"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="26"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="22"/>
+      <c r="B78" s="23"/>
       <c r="C78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="22"/>
-      <c r="B79" s="22"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="23"/>
       <c r="C79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
+      <c r="A80" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="22"/>
+      <c r="B80" s="23"/>
       <c r="C80" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="24"/>
+      <c r="B81" s="34"/>
       <c r="C81" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="27" t="s">
+      <c r="A82" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
@@ -1731,21 +1742,21 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B94" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C94" s="22"/>
+      <c r="B94" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94" s="23"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B95" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C95" s="22"/>
+      <c r="B95" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95" s="23"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
@@ -1754,16 +1765,16 @@
       <c r="B96" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C96" s="22"/>
+      <c r="C96" s="23"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C97" s="22"/>
+      <c r="C97" s="23"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
@@ -1772,75 +1783,75 @@
       <c r="B98" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C98" s="22"/>
+      <c r="C98" s="23"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B99" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C99" s="22"/>
+      <c r="B99" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" s="23"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="26" t="s">
+      <c r="A100" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="26"/>
+      <c r="B101" s="24"/>
       <c r="C101" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B102" s="22"/>
+      <c r="A102" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" s="23"/>
       <c r="C102" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B103" s="22"/>
+      <c r="A103" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="23"/>
       <c r="C103" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B104" s="22"/>
+      <c r="A104" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104" s="23"/>
       <c r="C104" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B105" s="22"/>
+      <c r="A105" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B105" s="23"/>
       <c r="C105" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="27" t="s">
+      <c r="A106" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="19" t="s">
@@ -1886,11 +1897,11 @@
       <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="29" t="s">
+      <c r="A114" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B114" s="30"/>
-      <c r="C114" s="31"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="22"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
@@ -1916,21 +1927,21 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B119" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C119" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="B119" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C119" s="23"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B120" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C120" s="22"/>
+      <c r="B120" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C120" s="23"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
@@ -1939,16 +1950,16 @@
       <c r="B121" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C121" s="22"/>
+      <c r="C121" s="23"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B122" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="C122" s="22"/>
+      <c r="B122" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C122" s="23"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
@@ -1957,62 +1968,62 @@
       <c r="B123" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C123" s="22"/>
+      <c r="C123" s="23"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B124" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="C124" s="22"/>
+      <c r="B124" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C124" s="23"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="26" t="s">
+      <c r="A125" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B125" s="26"/>
-      <c r="C125" s="26"/>
+      <c r="B125" s="24"/>
+      <c r="C125" s="24"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="26" t="s">
+      <c r="A126" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B126" s="26"/>
+      <c r="B126" s="24"/>
       <c r="C126" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B127" s="22"/>
+      <c r="A127" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B127" s="23"/>
       <c r="C127" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="22"/>
-      <c r="B128" s="22"/>
+      <c r="A128" s="23"/>
+      <c r="B128" s="23"/>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="27" t="s">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B129" s="27"/>
-      <c r="C129" s="27"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="26"/>
+      <c r="C129" s="26"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
         <v>10</v>
       </c>
@@ -2023,7 +2034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>1</v>
       </c>
@@ -2033,8 +2044,9 @@
       <c r="C132" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L132" s="35"/>
+    </row>
+    <row r="133" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>1</v>
       </c>
@@ -2045,7 +2057,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>1</v>
       </c>
@@ -2056,7 +2068,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>1</v>
       </c>
@@ -2067,19 +2079,19 @@
         <v>97</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="29" t="s">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A137" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B137" s="30"/>
-      <c r="C137" s="31"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="21"/>
+      <c r="C137" s="22"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="8" t="s">
         <v>10</v>
       </c>
@@ -2090,70 +2102,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="5"/>
       <c r="C139" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A130:C130"/>
-    <mergeCell ref="A137:C137"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A107:C107"/>
-    <mergeCell ref="A114:C114"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A50:C53"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A27:C30"/>
-    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A83:C83"/>
     <mergeCell ref="A66:C69"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="A10:C10"/>
@@ -2170,21 +2140,63 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A27:C30"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A50:C53"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A107:C107"/>
+    <mergeCell ref="A114:C114"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="A130:C130"/>
+    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>